<commit_message>
Update BOM_bus esp8266 sensor.xlsx
</commit_message>
<xml_diff>
--- a/BOM_bus esp8266 sensor.xlsx
+++ b/BOM_bus esp8266 sensor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d68ba8405bee2ea1/Documents/1962 GM PD4106-1227/projects/realdash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d68ba8405bee2ea1/Documents/1962 GM PD4106-1227/projects/ESPhome-engine-coolant-and-oil-pressure-sensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{30FA83D7-F16C-445C-A945-4B461A24E265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D38F1D89-77BA-40E5-95B9-4FB7FABBE268}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{30FA83D7-F16C-445C-A945-4B461A24E265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5916855F-08C8-4471-BA1E-1FD69CFAA837}"/>
   <bookViews>
-    <workbookView xWindow="2289" yWindow="-103" windowWidth="30728" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4149" windowWidth="22894" windowHeight="13594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_bus esp8266 sensor_2020-07-" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -179,19 +179,10 @@
     <t xml:space="preserve">https://amzn.to/32wXrgN </t>
   </si>
   <si>
-    <t>Project box</t>
-  </si>
-  <si>
     <t>REXQualis</t>
   </si>
   <si>
-    <t xml:space="preserve">https://amzn.to/2CqpfJ8 </t>
-  </si>
-  <si>
     <t>none</t>
-  </si>
-  <si>
-    <t>Onwon </t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1037,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1329,13 +1320,13 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
         <v>28</v>
@@ -1345,27 +1336,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="I12" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1375,9 +1346,8 @@
     <hyperlink ref="I9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="I10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="I11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="I12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>